<commit_message>
Final Student Management System with branch filter and UI
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,27 +463,189 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Yash</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>eve@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:28:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CSE-CyberSecurity</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>david@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:28:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CSE-ML</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>charlie@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:28:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CSE-DS</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>bob@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:27:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSE-AIML</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>alice@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:27:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sai</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CSE-AI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>sai@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:27:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Yashwanth</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>5A2</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>CSE</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>yash@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>06-02-2026 16:50:08</t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>06-02-2026 19:26:32</t>
         </is>
       </c>
     </row>

</xml_diff>